<commit_message>
updated with 0.5 m ball free moving test scenario
</commit_message>
<xml_diff>
--- a/docs/Testing/TestScenario.xlsx
+++ b/docs/Testing/TestScenario.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MSD2021_AutoRef\AutonomousReferee\docs\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCCD51D-27AA-4EA9-94A7-923739D83A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE35ADAE-B935-40FF-9D0E-0CAEAB31E6F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="FL_BallPlayerDistance" sheetId="1" r:id="rId1"/>
+    <sheet name="FL_BallFreeRollingAfterKick" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="40">
   <si>
     <t>Sl No.</t>
   </si>
@@ -120,6 +121,33 @@
   </si>
   <si>
     <t>One goal</t>
+  </si>
+  <si>
+    <t>Test Scenarios for FLs related to free rolling of ball of 0.5 m after kick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The second player takes/kicks the ball before the ball has rolled freely for 0.5 m after first player's kick </t>
+  </si>
+  <si>
+    <t>Task ID - 08.3.1.G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The first player itself takes/kicks the ball before the ball has rolled freely for 0.5 m after first kick </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The second player takes/kicks the ball after the ball has rolled freely for 0.5 m after first player's kick </t>
+  </si>
+  <si>
+    <t>No Rule violation</t>
+  </si>
+  <si>
+    <t>Task ID - 13.4.9</t>
+  </si>
+  <si>
+    <t>Task ID - 16.1.(3).E</t>
+  </si>
+  <si>
+    <t>Task ID - 17.1.(3).F</t>
   </si>
 </sst>
 </file>
@@ -408,24 +436,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -441,6 +451,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -505,6 +533,72 @@
         <a:xfrm>
           <a:off x="8828275" y="381000"/>
           <a:ext cx="4750564" cy="3032760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>57655</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>541019</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Soccer 101 — BYSA - Billerica Youth Soccer">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A72D89F4-0450-495E-B05A-EBC56DAA832A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8592055" y="415290"/>
+          <a:ext cx="4750564" cy="4078605"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -791,36 +885,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="25"/>
     </row>
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
     </row>
     <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -846,7 +940,7 @@
       <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="8" t="s">
@@ -931,7 +1025,7 @@
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="14" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -982,7 +1076,7 @@
       <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="14" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="3" t="s">
@@ -1010,33 +1104,33 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="21">
+      <c r="A14" s="15">
         <v>11</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="24" t="s">
+      <c r="D14" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="18" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="25"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="3"/>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="14" t="s">
         <v>29</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="25"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="3"/>
       <c r="C16" s="4" t="s">
         <v>30</v>
@@ -1053,4 +1147,340 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA2C8F73-11C5-4243-A38E-73F4227BB54B}">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="25"/>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>1</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>1</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>2</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>3</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>4</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <v>5</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>1</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>2</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <v>3</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>4</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="5">
+        <v>5</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="19"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="19"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>